<commit_message>
bugfix 21 - When the report contains accents in the text, the pdf generated doesn't contain the correct text.
</commit_message>
<xml_diff>
--- a/src/test/resources/golden/grid_report_golden.xlsx
+++ b/src/test/resources/golden/grid_report_golden.xlsx
@@ -13,42 +13,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="528">
-  <si>
-    <t>column 1</t>
-  </si>
-  <si>
-    <t>column 2</t>
-  </si>
-  <si>
-    <t>column 3</t>
-  </si>
-  <si>
-    <t>column 4</t>
-  </si>
-  <si>
-    <t>column 5</t>
-  </si>
-  <si>
-    <t>column 6</t>
-  </si>
-  <si>
-    <t>column 7</t>
-  </si>
-  <si>
-    <t>column 8</t>
-  </si>
-  <si>
-    <t>column 9</t>
-  </si>
-  <si>
-    <t>column 10</t>
-  </si>
-  <si>
-    <t>column 11</t>
-  </si>
-  <si>
-    <t>column 12</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="529">
+  <si>
+    <t>cólumn 1</t>
+  </si>
+  <si>
+    <t>cólumn 2</t>
+  </si>
+  <si>
+    <t>cólumn 3</t>
+  </si>
+  <si>
+    <t>cólumn 4</t>
+  </si>
+  <si>
+    <t>cólumn 5</t>
+  </si>
+  <si>
+    <t>cólumn 6</t>
+  </si>
+  <si>
+    <t>cólumn 7</t>
+  </si>
+  <si>
+    <t>cólumn 8</t>
+  </si>
+  <si>
+    <t>cólumn 9</t>
+  </si>
+  <si>
+    <t>cólumn 10</t>
+  </si>
+  <si>
+    <t>cólumn 11</t>
+  </si>
+  <si>
+    <t>cólumn 12</t>
   </si>
   <si>
     <t>1.1</t>
@@ -1569,34 +1569,37 @@
     <t>Second</t>
   </si>
   <si>
+    <t>Número</t>
+  </si>
+  <si>
+    <t>Third</t>
+  </si>
+  <si>
+    <t>Another one</t>
+  </si>
+  <si>
+    <t>Fourth</t>
+  </si>
+  <si>
+    <t>Last one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created at: </t>
+  </si>
+  <si>
+    <t>2021-12-01 10:01:01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created by: </t>
+  </si>
+  <si>
+    <t>My self</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Third: </t>
+  </si>
+  <si>
     <t>Another</t>
-  </si>
-  <si>
-    <t>Third</t>
-  </si>
-  <si>
-    <t>Another one</t>
-  </si>
-  <si>
-    <t>Fourth</t>
-  </si>
-  <si>
-    <t>Last one</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Created at: </t>
-  </si>
-  <si>
-    <t>2021-12-01 10:01:01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Created by: </t>
-  </si>
-  <si>
-    <t>My self</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Third: </t>
   </si>
 </sst>
 </file>
@@ -3730,7 +3733,7 @@
         <v>527</v>
       </c>
       <c r="B11" t="s">
-        <v>518</v>
+        <v>528</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bugfix 21 - When the report contains accents in the text, the pdf gen… (#22)
* bugfix 21 - When the report contains accents in the text, the pdf generated doesn't contain the correct text.

* bugfix 21 - Added pom version 1.8.2

Co-authored-by: pablo-gago <pgago@werfen.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/golden/grid_report_golden.xlsx
+++ b/src/test/resources/golden/grid_report_golden.xlsx
@@ -13,42 +13,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="528">
-  <si>
-    <t>column 1</t>
-  </si>
-  <si>
-    <t>column 2</t>
-  </si>
-  <si>
-    <t>column 3</t>
-  </si>
-  <si>
-    <t>column 4</t>
-  </si>
-  <si>
-    <t>column 5</t>
-  </si>
-  <si>
-    <t>column 6</t>
-  </si>
-  <si>
-    <t>column 7</t>
-  </si>
-  <si>
-    <t>column 8</t>
-  </si>
-  <si>
-    <t>column 9</t>
-  </si>
-  <si>
-    <t>column 10</t>
-  </si>
-  <si>
-    <t>column 11</t>
-  </si>
-  <si>
-    <t>column 12</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="529">
+  <si>
+    <t>cólumn 1</t>
+  </si>
+  <si>
+    <t>cólumn 2</t>
+  </si>
+  <si>
+    <t>cólumn 3</t>
+  </si>
+  <si>
+    <t>cólumn 4</t>
+  </si>
+  <si>
+    <t>cólumn 5</t>
+  </si>
+  <si>
+    <t>cólumn 6</t>
+  </si>
+  <si>
+    <t>cólumn 7</t>
+  </si>
+  <si>
+    <t>cólumn 8</t>
+  </si>
+  <si>
+    <t>cólumn 9</t>
+  </si>
+  <si>
+    <t>cólumn 10</t>
+  </si>
+  <si>
+    <t>cólumn 11</t>
+  </si>
+  <si>
+    <t>cólumn 12</t>
   </si>
   <si>
     <t>1.1</t>
@@ -1569,34 +1569,37 @@
     <t>Second</t>
   </si>
   <si>
+    <t>Número</t>
+  </si>
+  <si>
+    <t>Third</t>
+  </si>
+  <si>
+    <t>Another one</t>
+  </si>
+  <si>
+    <t>Fourth</t>
+  </si>
+  <si>
+    <t>Last one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created at: </t>
+  </si>
+  <si>
+    <t>2021-12-01 10:01:01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created by: </t>
+  </si>
+  <si>
+    <t>My self</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Third: </t>
+  </si>
+  <si>
     <t>Another</t>
-  </si>
-  <si>
-    <t>Third</t>
-  </si>
-  <si>
-    <t>Another one</t>
-  </si>
-  <si>
-    <t>Fourth</t>
-  </si>
-  <si>
-    <t>Last one</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Created at: </t>
-  </si>
-  <si>
-    <t>2021-12-01 10:01:01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Created by: </t>
-  </si>
-  <si>
-    <t>My self</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Third: </t>
   </si>
 </sst>
 </file>
@@ -3730,7 +3733,7 @@
         <v>527</v>
       </c>
       <c r="B11" t="s">
-        <v>518</v>
+        <v>528</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BEASW-17784: Updates test golden copies because little differences in new fonts library (tests still pases with the old ones: futureproof oriented).
</commit_message>
<xml_diff>
--- a/src/test/resources/golden/grid_report_golden.xlsx
+++ b/src/test/resources/golden/grid_report_golden.xlsx
@@ -1762,1902 +1762,1902 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="K2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="K2" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L2" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>25</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>31</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="K3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="K3" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L3" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="K4" t="s">
-        <v>22</v>
-      </c>
-      <c r="L4" t="s">
+      <c r="K4" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L4" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>44</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" t="s" s="0">
         <v>49</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" t="s" s="0">
         <v>50</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>51</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" t="s" s="0">
         <v>52</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" t="s" s="0">
         <v>53</v>
       </c>
-      <c r="K5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L5" t="s">
+      <c r="K5" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L5" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>54</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>56</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>57</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>58</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" t="s" s="0">
         <v>61</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" t="s" s="0">
         <v>62</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" t="s" s="0">
         <v>63</v>
       </c>
-      <c r="K6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L6" t="s">
+      <c r="K6" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L6" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>64</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>65</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>66</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>67</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" t="s" s="0">
         <v>68</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" t="s" s="0">
         <v>69</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" t="s" s="0">
         <v>71</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" t="s" s="0">
         <v>72</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" t="s" s="0">
         <v>73</v>
       </c>
-      <c r="K7" t="s">
-        <v>22</v>
-      </c>
-      <c r="L7" t="s">
+      <c r="K7" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L7" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>74</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>75</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>76</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>77</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" t="s" s="0">
         <v>78</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" t="s" s="0">
         <v>79</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" t="s" s="0">
         <v>80</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" t="s" s="0">
         <v>81</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" t="s" s="0">
         <v>82</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" t="s" s="0">
         <v>83</v>
       </c>
-      <c r="K8" t="s">
-        <v>22</v>
-      </c>
-      <c r="L8" t="s">
+      <c r="K8" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L8" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>84</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>85</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>86</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>87</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" t="s" s="0">
         <v>88</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" t="s" s="0">
         <v>89</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" t="s" s="0">
         <v>90</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" t="s" s="0">
         <v>91</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" t="s" s="0">
         <v>92</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" t="s" s="0">
         <v>93</v>
       </c>
-      <c r="K9" t="s">
-        <v>22</v>
-      </c>
-      <c r="L9" t="s">
+      <c r="K9" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L9" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>94</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>95</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>96</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>97</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" t="s" s="0">
         <v>99</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" t="s" s="0">
         <v>100</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" t="s" s="0">
         <v>101</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" t="s" s="0">
         <v>102</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" t="s" s="0">
         <v>103</v>
       </c>
-      <c r="K10" t="s">
-        <v>22</v>
-      </c>
-      <c r="L10" t="s">
+      <c r="K10" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L10" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s">
+      <c r="A11" t="s" s="0">
         <v>104</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="s" s="0">
         <v>107</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" t="s" s="0">
         <v>109</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" t="s" s="0">
         <v>110</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" t="s" s="0">
         <v>111</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" t="s" s="0">
         <v>112</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" t="s" s="0">
         <v>113</v>
       </c>
-      <c r="K11" t="s">
-        <v>22</v>
-      </c>
-      <c r="L11" t="s">
+      <c r="K11" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L11" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="s">
+      <c r="A12" t="s" s="0">
         <v>114</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" t="s" s="0">
         <v>115</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" t="s" s="0">
         <v>116</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" t="s" s="0">
         <v>117</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" t="s" s="0">
         <v>118</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" t="s" s="0">
         <v>119</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" t="s" s="0">
         <v>120</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" t="s" s="0">
         <v>121</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" t="s" s="0">
         <v>122</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" t="s" s="0">
         <v>123</v>
       </c>
-      <c r="K12" t="s">
-        <v>22</v>
-      </c>
-      <c r="L12" t="s">
+      <c r="K12" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L12" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s">
+      <c r="A13" t="s" s="0">
         <v>124</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" t="s" s="0">
         <v>125</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" t="s" s="0">
         <v>126</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" t="s" s="0">
         <v>127</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" t="s" s="0">
         <v>128</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" t="s" s="0">
         <v>129</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" t="s" s="0">
         <v>130</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" t="s" s="0">
         <v>131</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" t="s" s="0">
         <v>132</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" t="s" s="0">
         <v>133</v>
       </c>
-      <c r="K13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L13" t="s">
+      <c r="K13" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L13" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s">
+      <c r="A14" t="s" s="0">
         <v>134</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" t="s" s="0">
         <v>135</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" t="s" s="0">
         <v>136</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" t="s" s="0">
         <v>137</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" t="s" s="0">
         <v>138</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" t="s" s="0">
         <v>139</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" t="s" s="0">
         <v>140</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" t="s" s="0">
         <v>141</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" t="s" s="0">
         <v>142</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" t="s" s="0">
         <v>143</v>
       </c>
-      <c r="K14" t="s">
-        <v>22</v>
-      </c>
-      <c r="L14" t="s">
+      <c r="K14" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L14" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="s">
+      <c r="A15" t="s" s="0">
         <v>144</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" t="s" s="0">
         <v>145</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" t="s" s="0">
         <v>146</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" t="s" s="0">
         <v>147</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" t="s" s="0">
         <v>148</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" t="s" s="0">
         <v>149</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" t="s" s="0">
         <v>150</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" t="s" s="0">
         <v>151</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" t="s" s="0">
         <v>152</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" t="s" s="0">
         <v>153</v>
       </c>
-      <c r="K15" t="s">
-        <v>22</v>
-      </c>
-      <c r="L15" t="s">
+      <c r="K15" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L15" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="s">
+      <c r="A16" t="s" s="0">
         <v>154</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" t="s" s="0">
         <v>155</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" t="s" s="0">
         <v>156</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" t="s" s="0">
         <v>157</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" t="s" s="0">
         <v>158</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" t="s" s="0">
         <v>159</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" t="s" s="0">
         <v>160</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" t="s" s="0">
         <v>161</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" t="s" s="0">
         <v>162</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" t="s" s="0">
         <v>163</v>
       </c>
-      <c r="K16" t="s">
-        <v>22</v>
-      </c>
-      <c r="L16" t="s">
+      <c r="K16" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L16" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="s">
+      <c r="A17" t="s" s="0">
         <v>164</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" t="s" s="0">
         <v>165</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" t="s" s="0">
         <v>166</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" t="s" s="0">
         <v>167</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" t="s" s="0">
         <v>168</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" t="s" s="0">
         <v>169</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" t="s" s="0">
         <v>170</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" t="s" s="0">
         <v>171</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" t="s" s="0">
         <v>172</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" t="s" s="0">
         <v>173</v>
       </c>
-      <c r="K17" t="s">
-        <v>22</v>
-      </c>
-      <c r="L17" t="s">
+      <c r="K17" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L17" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="s">
+      <c r="A18" t="s" s="0">
         <v>174</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" t="s" s="0">
         <v>175</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" t="s" s="0">
         <v>176</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" t="s" s="0">
         <v>177</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" t="s" s="0">
         <v>178</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" t="s" s="0">
         <v>179</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" t="s" s="0">
         <v>180</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" t="s" s="0">
         <v>181</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18" t="s" s="0">
         <v>182</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" t="s" s="0">
         <v>183</v>
       </c>
-      <c r="K18" t="s">
-        <v>22</v>
-      </c>
-      <c r="L18" t="s">
+      <c r="K18" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L18" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="s">
+      <c r="A19" t="s" s="0">
         <v>184</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" t="s" s="0">
         <v>185</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" t="s" s="0">
         <v>186</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" t="s" s="0">
         <v>187</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" t="s" s="0">
         <v>188</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" t="s" s="0">
         <v>189</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" t="s" s="0">
         <v>190</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19" t="s" s="0">
         <v>191</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I19" t="s" s="0">
         <v>192</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" t="s" s="0">
         <v>193</v>
       </c>
-      <c r="K19" t="s">
-        <v>22</v>
-      </c>
-      <c r="L19" t="s">
+      <c r="K19" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L19" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="s">
+      <c r="A20" t="s" s="0">
         <v>194</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" t="s" s="0">
         <v>195</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" t="s" s="0">
         <v>196</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" t="s" s="0">
         <v>197</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" t="s" s="0">
         <v>198</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" t="s" s="0">
         <v>199</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" t="s" s="0">
         <v>200</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" t="s" s="0">
         <v>201</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20" t="s" s="0">
         <v>202</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J20" t="s" s="0">
         <v>203</v>
       </c>
-      <c r="K20" t="s">
-        <v>22</v>
-      </c>
-      <c r="L20" t="s">
+      <c r="K20" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L20" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="s">
+      <c r="A21" t="s" s="0">
         <v>204</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" t="s" s="0">
         <v>205</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" t="s" s="0">
         <v>206</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" t="s" s="0">
         <v>207</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" t="s" s="0">
         <v>208</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" t="s" s="0">
         <v>209</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" t="s" s="0">
         <v>210</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21" t="s" s="0">
         <v>211</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I21" t="s" s="0">
         <v>212</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J21" t="s" s="0">
         <v>213</v>
       </c>
-      <c r="K21" t="s">
-        <v>22</v>
-      </c>
-      <c r="L21" t="s">
+      <c r="K21" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L21" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="s">
+      <c r="A22" t="s" s="0">
         <v>214</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" t="s" s="0">
         <v>215</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" t="s" s="0">
         <v>216</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" t="s" s="0">
         <v>217</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" t="s" s="0">
         <v>218</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" t="s" s="0">
         <v>219</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" t="s" s="0">
         <v>220</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" t="s" s="0">
         <v>221</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I22" t="s" s="0">
         <v>222</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J22" t="s" s="0">
         <v>223</v>
       </c>
-      <c r="K22" t="s">
-        <v>22</v>
-      </c>
-      <c r="L22" t="s">
+      <c r="K22" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L22" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="s">
+      <c r="A23" t="s" s="0">
         <v>224</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" t="s" s="0">
         <v>225</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" t="s" s="0">
         <v>226</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" t="s" s="0">
         <v>227</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" t="s" s="0">
         <v>228</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" t="s" s="0">
         <v>229</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" t="s" s="0">
         <v>230</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" t="s" s="0">
         <v>231</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I23" t="s" s="0">
         <v>232</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J23" t="s" s="0">
         <v>233</v>
       </c>
-      <c r="K23" t="s">
-        <v>22</v>
-      </c>
-      <c r="L23" t="s">
+      <c r="K23" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L23" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="s">
+      <c r="A24" t="s" s="0">
         <v>234</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" t="s" s="0">
         <v>235</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" t="s" s="0">
         <v>236</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" t="s" s="0">
         <v>237</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" t="s" s="0">
         <v>238</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" t="s" s="0">
         <v>239</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" t="s" s="0">
         <v>240</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24" t="s" s="0">
         <v>241</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I24" t="s" s="0">
         <v>242</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J24" t="s" s="0">
         <v>243</v>
       </c>
-      <c r="K24" t="s">
-        <v>22</v>
-      </c>
-      <c r="L24" t="s">
+      <c r="K24" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L24" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="s">
+      <c r="A25" t="s" s="0">
         <v>244</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" t="s" s="0">
         <v>245</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" t="s" s="0">
         <v>246</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" t="s" s="0">
         <v>247</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" t="s" s="0">
         <v>248</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" t="s" s="0">
         <v>249</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" t="s" s="0">
         <v>250</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H25" t="s" s="0">
         <v>251</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I25" t="s" s="0">
         <v>252</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J25" t="s" s="0">
         <v>253</v>
       </c>
-      <c r="K25" t="s">
-        <v>22</v>
-      </c>
-      <c r="L25" t="s">
+      <c r="K25" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L25" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="s">
+      <c r="A26" t="s" s="0">
         <v>254</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" t="s" s="0">
         <v>255</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" t="s" s="0">
         <v>256</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" t="s" s="0">
         <v>257</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" t="s" s="0">
         <v>258</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26" t="s" s="0">
         <v>260</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26" t="s" s="0">
         <v>261</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I26" t="s" s="0">
         <v>262</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J26" t="s" s="0">
         <v>263</v>
       </c>
-      <c r="K26" t="s">
-        <v>22</v>
-      </c>
-      <c r="L26" t="s">
+      <c r="K26" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L26" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="s">
+      <c r="A27" t="s" s="0">
         <v>264</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" t="s" s="0">
         <v>265</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" t="s" s="0">
         <v>266</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" t="s" s="0">
         <v>267</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" t="s" s="0">
         <v>268</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" t="s" s="0">
         <v>269</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G27" t="s" s="0">
         <v>270</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H27" t="s" s="0">
         <v>271</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I27" t="s" s="0">
         <v>272</v>
       </c>
-      <c r="J27" t="s">
+      <c r="J27" t="s" s="0">
         <v>273</v>
       </c>
-      <c r="K27" t="s">
-        <v>22</v>
-      </c>
-      <c r="L27" t="s">
+      <c r="K27" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L27" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="s">
+      <c r="A28" t="s" s="0">
         <v>274</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" t="s" s="0">
         <v>275</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" t="s" s="0">
         <v>276</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" t="s" s="0">
         <v>277</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" t="s" s="0">
         <v>278</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" t="s" s="0">
         <v>279</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G28" t="s" s="0">
         <v>280</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H28" t="s" s="0">
         <v>281</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I28" t="s" s="0">
         <v>282</v>
       </c>
-      <c r="J28" t="s">
+      <c r="J28" t="s" s="0">
         <v>283</v>
       </c>
-      <c r="K28" t="s">
-        <v>22</v>
-      </c>
-      <c r="L28" t="s">
+      <c r="K28" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L28" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="s">
+      <c r="A29" t="s" s="0">
         <v>284</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" t="s" s="0">
         <v>285</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" t="s" s="0">
         <v>286</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" t="s" s="0">
         <v>287</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" t="s" s="0">
         <v>288</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" t="s" s="0">
         <v>289</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G29" t="s" s="0">
         <v>290</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H29" t="s" s="0">
         <v>291</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I29" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="J29" t="s">
+      <c r="J29" t="s" s="0">
         <v>293</v>
       </c>
-      <c r="K29" t="s">
-        <v>22</v>
-      </c>
-      <c r="L29" t="s">
+      <c r="K29" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L29" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="s">
+      <c r="A30" t="s" s="0">
         <v>294</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" t="s" s="0">
         <v>295</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" t="s" s="0">
         <v>296</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" t="s" s="0">
         <v>297</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" t="s" s="0">
         <v>298</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" t="s" s="0">
         <v>299</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" t="s" s="0">
         <v>300</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H30" t="s" s="0">
         <v>301</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I30" t="s" s="0">
         <v>302</v>
       </c>
-      <c r="J30" t="s">
+      <c r="J30" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="K30" t="s">
-        <v>22</v>
-      </c>
-      <c r="L30" t="s">
+      <c r="K30" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L30" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="s">
+      <c r="A31" t="s" s="0">
         <v>304</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" t="s" s="0">
         <v>305</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" t="s" s="0">
         <v>306</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" t="s" s="0">
         <v>307</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" t="s" s="0">
         <v>308</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" t="s" s="0">
         <v>309</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G31" t="s" s="0">
         <v>310</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H31" t="s" s="0">
         <v>311</v>
       </c>
-      <c r="I31" t="s">
+      <c r="I31" t="s" s="0">
         <v>312</v>
       </c>
-      <c r="J31" t="s">
+      <c r="J31" t="s" s="0">
         <v>313</v>
       </c>
-      <c r="K31" t="s">
-        <v>22</v>
-      </c>
-      <c r="L31" t="s">
+      <c r="K31" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L31" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="s">
+      <c r="A32" t="s" s="0">
         <v>314</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" t="s" s="0">
         <v>315</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" t="s" s="0">
         <v>316</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" t="s" s="0">
         <v>317</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" t="s" s="0">
         <v>318</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" t="s" s="0">
         <v>319</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G32" t="s" s="0">
         <v>320</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H32" t="s" s="0">
         <v>321</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I32" t="s" s="0">
         <v>322</v>
       </c>
-      <c r="J32" t="s">
+      <c r="J32" t="s" s="0">
         <v>323</v>
       </c>
-      <c r="K32" t="s">
-        <v>22</v>
-      </c>
-      <c r="L32" t="s">
+      <c r="K32" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L32" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="s">
+      <c r="A33" t="s" s="0">
         <v>324</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" t="s" s="0">
         <v>325</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" t="s" s="0">
         <v>326</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" t="s" s="0">
         <v>327</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" t="s" s="0">
         <v>328</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" t="s" s="0">
         <v>329</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G33" t="s" s="0">
         <v>330</v>
       </c>
-      <c r="H33" t="s">
+      <c r="H33" t="s" s="0">
         <v>331</v>
       </c>
-      <c r="I33" t="s">
+      <c r="I33" t="s" s="0">
         <v>332</v>
       </c>
-      <c r="J33" t="s">
+      <c r="J33" t="s" s="0">
         <v>333</v>
       </c>
-      <c r="K33" t="s">
-        <v>22</v>
-      </c>
-      <c r="L33" t="s">
+      <c r="K33" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L33" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="s">
+      <c r="A34" t="s" s="0">
         <v>334</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" t="s" s="0">
         <v>335</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" t="s" s="0">
         <v>336</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" t="s" s="0">
         <v>337</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" t="s" s="0">
         <v>338</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" t="s" s="0">
         <v>339</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G34" t="s" s="0">
         <v>340</v>
       </c>
-      <c r="H34" t="s">
+      <c r="H34" t="s" s="0">
         <v>341</v>
       </c>
-      <c r="I34" t="s">
+      <c r="I34" t="s" s="0">
         <v>342</v>
       </c>
-      <c r="J34" t="s">
+      <c r="J34" t="s" s="0">
         <v>343</v>
       </c>
-      <c r="K34" t="s">
-        <v>22</v>
-      </c>
-      <c r="L34" t="s">
+      <c r="K34" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L34" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="s">
+      <c r="A35" t="s" s="0">
         <v>344</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" t="s" s="0">
         <v>345</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" t="s" s="0">
         <v>346</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" t="s" s="0">
         <v>347</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" t="s" s="0">
         <v>348</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" t="s" s="0">
         <v>349</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G35" t="s" s="0">
         <v>350</v>
       </c>
-      <c r="H35" t="s">
+      <c r="H35" t="s" s="0">
         <v>351</v>
       </c>
-      <c r="I35" t="s">
+      <c r="I35" t="s" s="0">
         <v>352</v>
       </c>
-      <c r="J35" t="s">
+      <c r="J35" t="s" s="0">
         <v>353</v>
       </c>
-      <c r="K35" t="s">
-        <v>22</v>
-      </c>
-      <c r="L35" t="s">
+      <c r="K35" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L35" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="s">
+      <c r="A36" t="s" s="0">
         <v>354</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" t="s" s="0">
         <v>355</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" t="s" s="0">
         <v>356</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" t="s" s="0">
         <v>357</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" t="s" s="0">
         <v>358</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" t="s" s="0">
         <v>359</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G36" t="s" s="0">
         <v>360</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H36" t="s" s="0">
         <v>361</v>
       </c>
-      <c r="I36" t="s">
+      <c r="I36" t="s" s="0">
         <v>362</v>
       </c>
-      <c r="J36" t="s">
+      <c r="J36" t="s" s="0">
         <v>363</v>
       </c>
-      <c r="K36" t="s">
-        <v>22</v>
-      </c>
-      <c r="L36" t="s">
+      <c r="K36" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L36" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="s">
+      <c r="A37" t="s" s="0">
         <v>364</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" t="s" s="0">
         <v>365</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" t="s" s="0">
         <v>366</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" t="s" s="0">
         <v>367</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" t="s" s="0">
         <v>368</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37" t="s" s="0">
         <v>369</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G37" t="s" s="0">
         <v>370</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H37" t="s" s="0">
         <v>371</v>
       </c>
-      <c r="I37" t="s">
+      <c r="I37" t="s" s="0">
         <v>372</v>
       </c>
-      <c r="J37" t="s">
+      <c r="J37" t="s" s="0">
         <v>373</v>
       </c>
-      <c r="K37" t="s">
-        <v>22</v>
-      </c>
-      <c r="L37" t="s">
+      <c r="K37" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L37" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="s">
+      <c r="A38" t="s" s="0">
         <v>374</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" t="s" s="0">
         <v>375</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" t="s" s="0">
         <v>376</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" t="s" s="0">
         <v>377</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" t="s" s="0">
         <v>378</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" t="s" s="0">
         <v>379</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G38" t="s" s="0">
         <v>380</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H38" t="s" s="0">
         <v>381</v>
       </c>
-      <c r="I38" t="s">
+      <c r="I38" t="s" s="0">
         <v>382</v>
       </c>
-      <c r="J38" t="s">
+      <c r="J38" t="s" s="0">
         <v>383</v>
       </c>
-      <c r="K38" t="s">
-        <v>22</v>
-      </c>
-      <c r="L38" t="s">
+      <c r="K38" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L38" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="s">
+      <c r="A39" t="s" s="0">
         <v>384</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" t="s" s="0">
         <v>385</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" t="s" s="0">
         <v>386</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" t="s" s="0">
         <v>387</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" t="s" s="0">
         <v>388</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" t="s" s="0">
         <v>389</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G39" t="s" s="0">
         <v>390</v>
       </c>
-      <c r="H39" t="s">
+      <c r="H39" t="s" s="0">
         <v>391</v>
       </c>
-      <c r="I39" t="s">
+      <c r="I39" t="s" s="0">
         <v>392</v>
       </c>
-      <c r="J39" t="s">
+      <c r="J39" t="s" s="0">
         <v>393</v>
       </c>
-      <c r="K39" t="s">
-        <v>22</v>
-      </c>
-      <c r="L39" t="s">
+      <c r="K39" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L39" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="s">
+      <c r="A40" t="s" s="0">
         <v>394</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" t="s" s="0">
         <v>395</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" t="s" s="0">
         <v>396</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" t="s" s="0">
         <v>397</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" t="s" s="0">
         <v>398</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" t="s" s="0">
         <v>399</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G40" t="s" s="0">
         <v>400</v>
       </c>
-      <c r="H40" t="s">
+      <c r="H40" t="s" s="0">
         <v>401</v>
       </c>
-      <c r="I40" t="s">
+      <c r="I40" t="s" s="0">
         <v>402</v>
       </c>
-      <c r="J40" t="s">
+      <c r="J40" t="s" s="0">
         <v>403</v>
       </c>
-      <c r="K40" t="s">
-        <v>22</v>
-      </c>
-      <c r="L40" t="s">
+      <c r="K40" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L40" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="s">
+      <c r="A41" t="s" s="0">
         <v>404</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" t="s" s="0">
         <v>405</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" t="s" s="0">
         <v>406</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" t="s" s="0">
         <v>407</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" t="s" s="0">
         <v>408</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" t="s" s="0">
         <v>409</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G41" t="s" s="0">
         <v>410</v>
       </c>
-      <c r="H41" t="s">
+      <c r="H41" t="s" s="0">
         <v>411</v>
       </c>
-      <c r="I41" t="s">
+      <c r="I41" t="s" s="0">
         <v>412</v>
       </c>
-      <c r="J41" t="s">
+      <c r="J41" t="s" s="0">
         <v>413</v>
       </c>
-      <c r="K41" t="s">
-        <v>22</v>
-      </c>
-      <c r="L41" t="s">
+      <c r="K41" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L41" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="s">
+      <c r="A42" t="s" s="0">
         <v>414</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" t="s" s="0">
         <v>415</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" t="s" s="0">
         <v>416</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" t="s" s="0">
         <v>417</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" t="s" s="0">
         <v>418</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42" t="s" s="0">
         <v>419</v>
       </c>
-      <c r="G42" t="s">
+      <c r="G42" t="s" s="0">
         <v>420</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H42" t="s" s="0">
         <v>421</v>
       </c>
-      <c r="I42" t="s">
+      <c r="I42" t="s" s="0">
         <v>422</v>
       </c>
-      <c r="J42" t="s">
+      <c r="J42" t="s" s="0">
         <v>423</v>
       </c>
-      <c r="K42" t="s">
-        <v>22</v>
-      </c>
-      <c r="L42" t="s">
+      <c r="K42" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L42" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="s">
+      <c r="A43" t="s" s="0">
         <v>424</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" t="s" s="0">
         <v>425</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" t="s" s="0">
         <v>426</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" t="s" s="0">
         <v>427</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" t="s" s="0">
         <v>428</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43" t="s" s="0">
         <v>429</v>
       </c>
-      <c r="G43" t="s">
+      <c r="G43" t="s" s="0">
         <v>430</v>
       </c>
-      <c r="H43" t="s">
+      <c r="H43" t="s" s="0">
         <v>431</v>
       </c>
-      <c r="I43" t="s">
+      <c r="I43" t="s" s="0">
         <v>432</v>
       </c>
-      <c r="J43" t="s">
+      <c r="J43" t="s" s="0">
         <v>433</v>
       </c>
-      <c r="K43" t="s">
-        <v>22</v>
-      </c>
-      <c r="L43" t="s">
+      <c r="K43" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L43" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="s">
+      <c r="A44" t="s" s="0">
         <v>434</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" t="s" s="0">
         <v>435</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" t="s" s="0">
         <v>436</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" t="s" s="0">
         <v>437</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" t="s" s="0">
         <v>438</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" t="s" s="0">
         <v>439</v>
       </c>
-      <c r="G44" t="s">
+      <c r="G44" t="s" s="0">
         <v>440</v>
       </c>
-      <c r="H44" t="s">
+      <c r="H44" t="s" s="0">
         <v>441</v>
       </c>
-      <c r="I44" t="s">
+      <c r="I44" t="s" s="0">
         <v>442</v>
       </c>
-      <c r="J44" t="s">
+      <c r="J44" t="s" s="0">
         <v>443</v>
       </c>
-      <c r="K44" t="s">
-        <v>22</v>
-      </c>
-      <c r="L44" t="s">
+      <c r="K44" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L44" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="s">
+      <c r="A45" t="s" s="0">
         <v>444</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" t="s" s="0">
         <v>445</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" t="s" s="0">
         <v>446</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" t="s" s="0">
         <v>447</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" t="s" s="0">
         <v>448</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F45" t="s" s="0">
         <v>449</v>
       </c>
-      <c r="G45" t="s">
+      <c r="G45" t="s" s="0">
         <v>450</v>
       </c>
-      <c r="H45" t="s">
+      <c r="H45" t="s" s="0">
         <v>451</v>
       </c>
-      <c r="I45" t="s">
+      <c r="I45" t="s" s="0">
         <v>452</v>
       </c>
-      <c r="J45" t="s">
+      <c r="J45" t="s" s="0">
         <v>453</v>
       </c>
-      <c r="K45" t="s">
-        <v>22</v>
-      </c>
-      <c r="L45" t="s">
+      <c r="K45" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L45" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="s">
+      <c r="A46" t="s" s="0">
         <v>454</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" t="s" s="0">
         <v>455</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" t="s" s="0">
         <v>456</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" t="s" s="0">
         <v>457</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" t="s" s="0">
         <v>458</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F46" t="s" s="0">
         <v>459</v>
       </c>
-      <c r="G46" t="s">
+      <c r="G46" t="s" s="0">
         <v>460</v>
       </c>
-      <c r="H46" t="s">
+      <c r="H46" t="s" s="0">
         <v>461</v>
       </c>
-      <c r="I46" t="s">
+      <c r="I46" t="s" s="0">
         <v>462</v>
       </c>
-      <c r="J46" t="s">
+      <c r="J46" t="s" s="0">
         <v>463</v>
       </c>
-      <c r="K46" t="s">
-        <v>22</v>
-      </c>
-      <c r="L46" t="s">
+      <c r="K46" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L46" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="s">
+      <c r="A47" t="s" s="0">
         <v>464</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" t="s" s="0">
         <v>465</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" t="s" s="0">
         <v>466</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" t="s" s="0">
         <v>467</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" t="s" s="0">
         <v>468</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F47" t="s" s="0">
         <v>469</v>
       </c>
-      <c r="G47" t="s">
+      <c r="G47" t="s" s="0">
         <v>470</v>
       </c>
-      <c r="H47" t="s">
+      <c r="H47" t="s" s="0">
         <v>471</v>
       </c>
-      <c r="I47" t="s">
+      <c r="I47" t="s" s="0">
         <v>472</v>
       </c>
-      <c r="J47" t="s">
+      <c r="J47" t="s" s="0">
         <v>473</v>
       </c>
-      <c r="K47" t="s">
-        <v>22</v>
-      </c>
-      <c r="L47" t="s">
+      <c r="K47" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L47" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="s">
+      <c r="A48" t="s" s="0">
         <v>474</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" t="s" s="0">
         <v>475</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" t="s" s="0">
         <v>476</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" t="s" s="0">
         <v>477</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" t="s" s="0">
         <v>478</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F48" t="s" s="0">
         <v>479</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G48" t="s" s="0">
         <v>480</v>
       </c>
-      <c r="H48" t="s">
+      <c r="H48" t="s" s="0">
         <v>481</v>
       </c>
-      <c r="I48" t="s">
+      <c r="I48" t="s" s="0">
         <v>482</v>
       </c>
-      <c r="J48" t="s">
+      <c r="J48" t="s" s="0">
         <v>483</v>
       </c>
-      <c r="K48" t="s">
-        <v>22</v>
-      </c>
-      <c r="L48" t="s">
+      <c r="K48" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L48" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="s">
+      <c r="A49" t="s" s="0">
         <v>484</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" t="s" s="0">
         <v>485</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" t="s" s="0">
         <v>486</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" t="s" s="0">
         <v>487</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" t="s" s="0">
         <v>488</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F49" t="s" s="0">
         <v>489</v>
       </c>
-      <c r="G49" t="s">
+      <c r="G49" t="s" s="0">
         <v>490</v>
       </c>
-      <c r="H49" t="s">
+      <c r="H49" t="s" s="0">
         <v>491</v>
       </c>
-      <c r="I49" t="s">
+      <c r="I49" t="s" s="0">
         <v>492</v>
       </c>
-      <c r="J49" t="s">
+      <c r="J49" t="s" s="0">
         <v>493</v>
       </c>
-      <c r="K49" t="s">
-        <v>22</v>
-      </c>
-      <c r="L49" t="s">
+      <c r="K49" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L49" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="s">
+      <c r="A50" t="s" s="0">
         <v>494</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" t="s" s="0">
         <v>495</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" t="s" s="0">
         <v>496</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" t="s" s="0">
         <v>497</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50" t="s" s="0">
         <v>498</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F50" t="s" s="0">
         <v>499</v>
       </c>
-      <c r="G50" t="s">
+      <c r="G50" t="s" s="0">
         <v>500</v>
       </c>
-      <c r="H50" t="s">
+      <c r="H50" t="s" s="0">
         <v>501</v>
       </c>
-      <c r="I50" t="s">
+      <c r="I50" t="s" s="0">
         <v>502</v>
       </c>
-      <c r="J50" t="s">
+      <c r="J50" t="s" s="0">
         <v>503</v>
       </c>
-      <c r="K50" t="s">
-        <v>22</v>
-      </c>
-      <c r="L50" t="s">
+      <c r="K50" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L50" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="s">
+      <c r="A51" t="s" s="0">
         <v>504</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" t="s" s="0">
         <v>505</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" t="s" s="0">
         <v>506</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" t="s" s="0">
         <v>507</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" t="s" s="0">
         <v>508</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F51" t="s" s="0">
         <v>509</v>
       </c>
-      <c r="G51" t="s">
+      <c r="G51" t="s" s="0">
         <v>510</v>
       </c>
-      <c r="H51" t="s">
+      <c r="H51" t="s" s="0">
         <v>511</v>
       </c>
-      <c r="I51" t="s">
+      <c r="I51" t="s" s="0">
         <v>512</v>
       </c>
-      <c r="J51" t="s">
+      <c r="J51" t="s" s="0">
         <v>513</v>
       </c>
-      <c r="K51" t="s">
-        <v>22</v>
-      </c>
-      <c r="L51" t="s">
+      <c r="K51" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L51" t="s" s="0">
         <v>23</v>
       </c>
     </row>
@@ -3675,64 +3675,64 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>514</v>
       </c>
-      <c r="C1"/>
+      <c r="C1" s="0"/>
     </row>
     <row r="3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>515</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>516</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>517</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>518</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>519</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>520</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>521</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>522</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>523</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>524</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>525</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>526</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s">
+      <c r="A11" t="s" s="0">
         <v>527</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" t="s" s="0">
         <v>528</v>
       </c>
     </row>

</xml_diff>